<commit_message>
Updated Build of materials.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>PART</t>
   </si>
@@ -43,13 +43,19 @@
     <t>EA</t>
   </si>
   <si>
-    <t>Steel Rods</t>
+    <t>Steel Rods 08x375 mm</t>
   </si>
   <si>
     <t>McMaster-CARR</t>
   </si>
   <si>
-    <t>Threaded Rods</t>
+    <t>Steel Rods 08x341 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel Rods 08x320 mm </t>
+  </si>
+  <si>
+    <t>M5 Threaded Rods</t>
   </si>
   <si>
     <t>M3 Hex Nut</t>
@@ -58,7 +64,7 @@
     <t>PK</t>
   </si>
   <si>
-    <t>M3 Nylon-Insert Locknut</t>
+    <t>M3 Nylon-Locknut</t>
   </si>
   <si>
     <t>M3 Flat Washer</t>
@@ -97,6 +103,9 @@
     <t>Mechanical Endstop</t>
   </si>
   <si>
+    <t>Easy RepRap</t>
+  </si>
+  <si>
     <t>14 Gauge Black Wire</t>
   </si>
   <si>
@@ -124,9 +133,6 @@
     <t>GT2 belt and pulley set</t>
   </si>
   <si>
-    <t>Easy RepRap</t>
-  </si>
-  <si>
     <t>MK8 Drive Gear</t>
   </si>
   <si>
@@ -143,6 +149,12 @@
   </si>
   <si>
     <t>SE 784EC Digital Caliper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 Stud Thermistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D CAM </t>
   </si>
 </sst>
 </file>
@@ -163,12 +175,12 @@
     </font>
     <font/>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <sz val="9.0"/>
       <color rgb="FF333333"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -245,10 +257,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -345,7 +357,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="11" t="str">
-        <f t="shared" ref="G2:G3" si="1">D2*E2</f>
+        <f t="shared" ref="G2:G28" si="1">D2*E2</f>
         <v>$41.44</v>
       </c>
     </row>
@@ -357,9 +369,11 @@
         <v>11</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="11"/>
+      <c r="D3" s="9">
+        <v>0.0</v>
+      </c>
       <c r="E3" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>9</v>
@@ -373,12 +387,23 @@
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$0.00</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
@@ -387,276 +412,288 @@
       <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="str">
+      <c r="D5" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="13" t="str">
         <f>HYPERLINK("http://www.mcmaster.com/#90591a250/=xst4ec","90591A250")</f>
         <v>90591A250</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D7" s="14">
         <v>2.06</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E7" s="10">
         <v>1.0</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="11" t="str">
-        <f t="shared" ref="G5:G25" si="2">D5*E5</f>
+      <c r="F7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$2.06</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14" t="str">
+      <c r="C8" s="13" t="str">
         <f>HYPERLINK("http://www.mcmaster.com/#90576a102/=xsshuh","90576A102")</f>
         <v>90576A102</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D8" s="9">
         <v>3.27</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E8" s="10">
         <v>1.0</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="F8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$3.27</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14" t="str">
+      <c r="C9" s="13" t="str">
         <f>HYPERLINK("http://www.mcmaster.com/#91166a210/=xsshhz","91166A210")</f>
         <v>91166A210</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D9" s="9">
         <v>1.61</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E9" s="10">
         <v>1.0</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="F9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$1.61</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9">
+    <row r="10">
+      <c r="A10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9">
         <v>8.0</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E10" s="10">
         <v>2.0</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="G10" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$16.00</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="14" t="str">
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="13" t="str">
         <f>HYPERLINK("http://www.vxb.com/page/bearings/PROD/8mmLinearMotionSystems/Kit179960","Kit179960")</f>
         <v>Kit179960</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D11" s="9">
         <v>24.95</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E11" s="10">
         <v>1.0</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="F11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$24.95</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$0.00</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$0.00</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="14" t="str">
+      <c r="B13" s="16"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="13" t="str">
         <f>HYPERLINK("http://www.panucatt.com/azteeg_X5_mini_reprap_3d_printer_controller_p/ax5mini.htm","AX5MINI")</f>
         <v>AX5MINI</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D14" s="9">
         <v>109.0</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E14" s="10">
         <v>1.0</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="G14" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$109.00</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9">
-        <v>5.39</v>
-      </c>
-      <c r="E13" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$5.39</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$0.00</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="9">
-        <v>0.22</v>
+        <v>5.39</v>
       </c>
       <c r="E15" s="10">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G15" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$2.20</v>
+        <f t="shared" si="1"/>
+        <v>$5.39</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="C16" s="13" t="str">
+        <f>HYPERLINK("http://www.amazon.com/gp/product/B00G2E6UZC/ref=pd_lpo_sbs_dp_ss_1?pf_rd_p=1944687502&amp;pf_rd_s=lpo-top-stripe-1&amp;pf_rd_t=201&amp;pf_rd_i=B00EVOTVY2&amp;pf_rd_m=ATVPDKIKX0DER&amp;pf_rd_r=0MEB5ZHP3EWNKZSQXCGF","ES3RL")</f>
+        <v>ES3RL</v>
+      </c>
       <c r="D16" s="9">
-        <v>0.22</v>
+        <v>8.99</v>
       </c>
       <c r="E16" s="10">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G16" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$2.20</v>
+        <f t="shared" si="1"/>
+        <v>$8.99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9">
-        <v>46.0</v>
+        <v>0.22</v>
       </c>
       <c r="E17" s="10">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G17" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$46.00</v>
+        <f t="shared" si="1"/>
+        <v>$2.20</v>
       </c>
     </row>
     <row r="18">
@@ -664,21 +701,21 @@
         <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9">
-        <v>79.0</v>
+        <v>0.22</v>
       </c>
       <c r="E18" s="10">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G18" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$79.00</v>
+        <f t="shared" si="1"/>
+        <v>$2.20</v>
       </c>
     </row>
     <row r="19">
@@ -686,49 +723,43 @@
         <v>35</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="14" t="str">
-        <f>HYPERLINK("http://www.3dmakerworld.com/nema17-stepper-motor","1124090")</f>
-        <v>1124090</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="9">
-        <v>14.5</v>
+        <v>46.0</v>
       </c>
       <c r="E19" s="10">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$72.50</v>
+        <f t="shared" si="1"/>
+        <v>$46.00</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="14" t="str">
-        <f>HYPERLINK("http://www.amazon.com/Easy-RepRap-Pulley-Printers-MendelMax/dp/B00ICM8ATG/ref=sr_1_2?s=industrial&amp;ie=UTF8&amp;qid=1435992613&amp;sr=1-2&amp;keywords=GT2+Belt+Pulley#product-description-iframe","GT2-20T")</f>
-        <v>GT2-20T</v>
-      </c>
+      <c r="C20" s="8"/>
       <c r="D20" s="9">
-        <v>17.99</v>
+        <v>79.0</v>
       </c>
       <c r="E20" s="10">
         <v>1.0</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G20" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$17.99</v>
+        <f t="shared" si="1"/>
+        <v>$79.00</v>
       </c>
     </row>
     <row r="21">
@@ -736,64 +767,64 @@
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="13" t="str">
+        <f>HYPERLINK("http://www.3dmakerworld.com/nema17-stepper-motor","1124090")</f>
+        <v>1124090</v>
+      </c>
+      <c r="D21" s="9">
+        <v>14.5</v>
+      </c>
+      <c r="E21" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$72.50</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="14" t="str">
+      <c r="B22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="13" t="str">
+        <f>HYPERLINK("http://www.amazon.com/Easy-RepRap-Pulley-Printers-MendelMax/dp/B00ICM8ATG/ref=sr_1_2?s=industrial&amp;ie=UTF8&amp;qid=1435992613&amp;sr=1-2&amp;keywords=GT2+Belt+Pulley#product-description-iframe","GT2-20T")</f>
+        <v>GT2-20T</v>
+      </c>
+      <c r="D22" s="9">
+        <v>17.99</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$17.99</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="13" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00THZK97I?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","MK8GEAR")</f>
         <v>MK8GEAR</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D23" s="9">
         <v>7.95</v>
-      </c>
-      <c r="E21" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$7.95</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="14" t="str">
-        <f>HYPERLINK("http://www.amazon.com/gp/product/B00THZJE8S?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","ABP01KIT2")</f>
-        <v>ABP01KIT2</v>
-      </c>
-      <c r="D22" s="9">
-        <v>45.95</v>
-      </c>
-      <c r="E22" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$45.95</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="14" t="str">
-        <f>HYPERLINK("http://www.amazon.com/gp/product/B0012EI6KE?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o04_s00","P007-010")</f>
-        <v>P007-010</v>
-      </c>
-      <c r="D23" s="9">
-        <v>11.81</v>
       </c>
       <c r="E23" s="10">
         <v>1.0</v>
@@ -802,8 +833,8 @@
         <v>9</v>
       </c>
       <c r="G23" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$11.81</v>
+        <f t="shared" si="1"/>
+        <v>$7.95</v>
       </c>
     </row>
     <row r="24">
@@ -811,14 +842,14 @@
         <v>42</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="14" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/WD-40-3-in-1-3-oz-Multi-Purpose-Precision-Lubricant-Liquid-Oil-100353/203732387?keyword=3+in+1+multipurpose+oil","203732387")</f>
-        <v>203732387</v>
+        <v>41</v>
+      </c>
+      <c r="C24" s="13" t="str">
+        <f>HYPERLINK("http://www.amazon.com/gp/product/B00THZJE8S?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","ABP01KIT2")</f>
+        <v>ABP01KIT2</v>
       </c>
       <c r="D24" s="9">
-        <v>2.28</v>
+        <v>45.95</v>
       </c>
       <c r="E24" s="10">
         <v>1.0</v>
@@ -827,8 +858,8 @@
         <v>9</v>
       </c>
       <c r="G24" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>$2.28</v>
+        <f t="shared" si="1"/>
+        <v>$45.95</v>
       </c>
     </row>
     <row r="25">
@@ -836,48 +867,100 @@
         <v>43</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="14" t="str">
+        <v>28</v>
+      </c>
+      <c r="C25" s="13" t="str">
+        <f>HYPERLINK("http://www.amazon.com/gp/product/B0012EI6KE?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o04_s00","P007-010")</f>
+        <v>P007-010</v>
+      </c>
+      <c r="D25" s="9">
+        <v>11.81</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$11.81</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="13" t="str">
+        <f>HYPERLINK("http://www.homedepot.com/p/WD-40-3-in-1-3-oz-Multi-Purpose-Precision-Lubricant-Liquid-Oil-100353/203732387?keyword=3+in+1+multipurpose+oil","203732387")</f>
+        <v>203732387</v>
+      </c>
+      <c r="D26" s="9">
+        <v>2.28</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$2.28</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="13" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002JFMIO?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o08_s02","784EC")</f>
         <v>784EC</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D27" s="9">
         <v>11.75</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E27" s="10">
         <v>1.0</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="G27" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>$11.75</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="16"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="16"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-    </row>
     <row r="28">
-      <c r="B28" s="16"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="13" t="str">
+        <f>HYPERLINK("http://www.amazon.com/gp/product/B00THZJIY8?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o00_s00","HEXTHERM")</f>
+        <v>HEXTHERM</v>
+      </c>
+      <c r="D28" s="9">
+        <v>11.95</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>$11.95</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="16"/>
@@ -901,10 +984,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="11" t="str">
-        <f>SUM(G2:G30)</f>
-        <v>$503.35</v>
-      </c>
+      <c r="G31" s="8"/>
     </row>
     <row r="32">
       <c r="B32" s="16"/>
@@ -920,7 +1000,10 @@
       <c r="D33" s="11"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
+      <c r="G33" s="11" t="str">
+        <f>SUM(G2:G32)</f>
+        <v>$524.29</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="16"/>
@@ -7586,1109 +7669,23 @@
       <c r="F866" s="8"/>
       <c r="G866" s="8"/>
     </row>
-    <row r="867">
-      <c r="B867" s="16"/>
-      <c r="C867" s="8"/>
-      <c r="D867" s="11"/>
-      <c r="E867" s="8"/>
-      <c r="F867" s="8"/>
-      <c r="G867" s="8"/>
-    </row>
-    <row r="868">
-      <c r="B868" s="16"/>
-      <c r="C868" s="8"/>
-      <c r="D868" s="11"/>
-      <c r="E868" s="8"/>
-      <c r="F868" s="8"/>
-      <c r="G868" s="8"/>
-    </row>
-    <row r="869">
-      <c r="B869" s="16"/>
-      <c r="C869" s="8"/>
-      <c r="D869" s="11"/>
-      <c r="E869" s="8"/>
-      <c r="F869" s="8"/>
-      <c r="G869" s="8"/>
-    </row>
-    <row r="870">
-      <c r="B870" s="16"/>
-      <c r="C870" s="8"/>
-      <c r="D870" s="11"/>
-      <c r="E870" s="8"/>
-      <c r="F870" s="8"/>
-      <c r="G870" s="8"/>
-    </row>
-    <row r="871">
-      <c r="B871" s="16"/>
-      <c r="C871" s="8"/>
-      <c r="D871" s="11"/>
-      <c r="E871" s="8"/>
-      <c r="F871" s="8"/>
-      <c r="G871" s="8"/>
-    </row>
-    <row r="872">
-      <c r="B872" s="16"/>
-      <c r="C872" s="8"/>
-      <c r="D872" s="11"/>
-      <c r="E872" s="8"/>
-      <c r="F872" s="8"/>
-      <c r="G872" s="8"/>
-    </row>
-    <row r="873">
-      <c r="B873" s="16"/>
-      <c r="C873" s="8"/>
-      <c r="D873" s="11"/>
-      <c r="E873" s="8"/>
-      <c r="F873" s="8"/>
-      <c r="G873" s="8"/>
-    </row>
-    <row r="874">
-      <c r="B874" s="16"/>
-      <c r="C874" s="8"/>
-      <c r="D874" s="11"/>
-      <c r="E874" s="8"/>
-      <c r="F874" s="8"/>
-      <c r="G874" s="8"/>
-    </row>
-    <row r="875">
-      <c r="B875" s="16"/>
-      <c r="C875" s="8"/>
-      <c r="D875" s="11"/>
-      <c r="E875" s="8"/>
-      <c r="F875" s="8"/>
-      <c r="G875" s="8"/>
-    </row>
-    <row r="876">
-      <c r="B876" s="16"/>
-      <c r="C876" s="8"/>
-      <c r="D876" s="11"/>
-      <c r="E876" s="8"/>
-      <c r="F876" s="8"/>
-      <c r="G876" s="8"/>
-    </row>
-    <row r="877">
-      <c r="B877" s="16"/>
-      <c r="C877" s="8"/>
-      <c r="D877" s="11"/>
-      <c r="E877" s="8"/>
-      <c r="F877" s="8"/>
-      <c r="G877" s="8"/>
-    </row>
-    <row r="878">
-      <c r="B878" s="16"/>
-      <c r="C878" s="8"/>
-      <c r="D878" s="11"/>
-      <c r="E878" s="8"/>
-      <c r="F878" s="8"/>
-      <c r="G878" s="8"/>
-    </row>
-    <row r="879">
-      <c r="B879" s="16"/>
-      <c r="C879" s="8"/>
-      <c r="D879" s="11"/>
-      <c r="E879" s="8"/>
-      <c r="F879" s="8"/>
-      <c r="G879" s="8"/>
-    </row>
-    <row r="880">
-      <c r="B880" s="16"/>
-      <c r="C880" s="8"/>
-      <c r="D880" s="11"/>
-      <c r="E880" s="8"/>
-      <c r="F880" s="8"/>
-      <c r="G880" s="8"/>
-    </row>
-    <row r="881">
-      <c r="B881" s="16"/>
-      <c r="C881" s="8"/>
-      <c r="D881" s="11"/>
-      <c r="E881" s="8"/>
-      <c r="F881" s="8"/>
-      <c r="G881" s="8"/>
-    </row>
-    <row r="882">
-      <c r="B882" s="16"/>
-      <c r="C882" s="8"/>
-      <c r="D882" s="11"/>
-      <c r="E882" s="8"/>
-      <c r="F882" s="8"/>
-      <c r="G882" s="8"/>
-    </row>
-    <row r="883">
-      <c r="B883" s="16"/>
-      <c r="C883" s="8"/>
-      <c r="D883" s="11"/>
-      <c r="E883" s="8"/>
-      <c r="F883" s="8"/>
-      <c r="G883" s="8"/>
-    </row>
-    <row r="884">
-      <c r="B884" s="16"/>
-      <c r="C884" s="8"/>
-      <c r="D884" s="11"/>
-      <c r="E884" s="8"/>
-      <c r="F884" s="8"/>
-      <c r="G884" s="8"/>
-    </row>
-    <row r="885">
-      <c r="B885" s="16"/>
-      <c r="C885" s="8"/>
-      <c r="D885" s="11"/>
-      <c r="E885" s="8"/>
-      <c r="F885" s="8"/>
-      <c r="G885" s="8"/>
-    </row>
-    <row r="886">
-      <c r="B886" s="16"/>
-      <c r="C886" s="8"/>
-      <c r="D886" s="11"/>
-      <c r="E886" s="8"/>
-      <c r="F886" s="8"/>
-      <c r="G886" s="8"/>
-    </row>
-    <row r="887">
-      <c r="B887" s="16"/>
-      <c r="C887" s="8"/>
-      <c r="D887" s="11"/>
-      <c r="E887" s="8"/>
-      <c r="F887" s="8"/>
-      <c r="G887" s="8"/>
-    </row>
-    <row r="888">
-      <c r="B888" s="16"/>
-      <c r="C888" s="8"/>
-      <c r="D888" s="11"/>
-      <c r="E888" s="8"/>
-      <c r="F888" s="8"/>
-      <c r="G888" s="8"/>
-    </row>
-    <row r="889">
-      <c r="B889" s="16"/>
-      <c r="C889" s="8"/>
-      <c r="D889" s="11"/>
-      <c r="E889" s="8"/>
-      <c r="F889" s="8"/>
-      <c r="G889" s="8"/>
-    </row>
-    <row r="890">
-      <c r="B890" s="16"/>
-      <c r="C890" s="8"/>
-      <c r="D890" s="11"/>
-      <c r="E890" s="8"/>
-      <c r="F890" s="8"/>
-      <c r="G890" s="8"/>
-    </row>
-    <row r="891">
-      <c r="B891" s="16"/>
-      <c r="C891" s="8"/>
-      <c r="D891" s="11"/>
-      <c r="E891" s="8"/>
-      <c r="F891" s="8"/>
-      <c r="G891" s="8"/>
-    </row>
-    <row r="892">
-      <c r="B892" s="16"/>
-      <c r="C892" s="8"/>
-      <c r="D892" s="11"/>
-      <c r="E892" s="8"/>
-      <c r="F892" s="8"/>
-      <c r="G892" s="8"/>
-    </row>
-    <row r="893">
-      <c r="B893" s="16"/>
-      <c r="C893" s="8"/>
-      <c r="D893" s="11"/>
-      <c r="E893" s="8"/>
-      <c r="F893" s="8"/>
-      <c r="G893" s="8"/>
-    </row>
-    <row r="894">
-      <c r="B894" s="16"/>
-      <c r="C894" s="8"/>
-      <c r="D894" s="11"/>
-      <c r="E894" s="8"/>
-      <c r="F894" s="8"/>
-      <c r="G894" s="8"/>
-    </row>
-    <row r="895">
-      <c r="B895" s="16"/>
-      <c r="C895" s="8"/>
-      <c r="D895" s="11"/>
-      <c r="E895" s="8"/>
-      <c r="F895" s="8"/>
-      <c r="G895" s="8"/>
-    </row>
-    <row r="896">
-      <c r="B896" s="16"/>
-      <c r="C896" s="8"/>
-      <c r="D896" s="11"/>
-      <c r="E896" s="8"/>
-      <c r="F896" s="8"/>
-      <c r="G896" s="8"/>
-    </row>
-    <row r="897">
-      <c r="B897" s="16"/>
-      <c r="C897" s="8"/>
-      <c r="D897" s="11"/>
-      <c r="E897" s="8"/>
-      <c r="F897" s="8"/>
-      <c r="G897" s="8"/>
-    </row>
-    <row r="898">
-      <c r="B898" s="16"/>
-      <c r="C898" s="8"/>
-      <c r="D898" s="11"/>
-      <c r="E898" s="8"/>
-      <c r="F898" s="8"/>
-      <c r="G898" s="8"/>
-    </row>
-    <row r="899">
-      <c r="B899" s="16"/>
-      <c r="C899" s="8"/>
-      <c r="D899" s="11"/>
-      <c r="E899" s="8"/>
-      <c r="F899" s="8"/>
-      <c r="G899" s="8"/>
-    </row>
-    <row r="900">
-      <c r="B900" s="16"/>
-      <c r="C900" s="8"/>
-      <c r="D900" s="11"/>
-      <c r="E900" s="8"/>
-      <c r="F900" s="8"/>
-      <c r="G900" s="8"/>
-    </row>
-    <row r="901">
-      <c r="B901" s="16"/>
-      <c r="C901" s="8"/>
-      <c r="D901" s="11"/>
-      <c r="E901" s="8"/>
-      <c r="F901" s="8"/>
-      <c r="G901" s="8"/>
-    </row>
-    <row r="902">
-      <c r="B902" s="16"/>
-      <c r="C902" s="8"/>
-      <c r="D902" s="11"/>
-      <c r="E902" s="8"/>
-      <c r="F902" s="8"/>
-      <c r="G902" s="8"/>
-    </row>
-    <row r="903">
-      <c r="B903" s="16"/>
-      <c r="C903" s="8"/>
-      <c r="D903" s="11"/>
-      <c r="E903" s="8"/>
-      <c r="F903" s="8"/>
-      <c r="G903" s="8"/>
-    </row>
-    <row r="904">
-      <c r="B904" s="16"/>
-      <c r="C904" s="8"/>
-      <c r="D904" s="11"/>
-      <c r="E904" s="8"/>
-      <c r="F904" s="8"/>
-      <c r="G904" s="8"/>
-    </row>
-    <row r="905">
-      <c r="B905" s="16"/>
-      <c r="C905" s="8"/>
-      <c r="D905" s="11"/>
-      <c r="E905" s="8"/>
-      <c r="F905" s="8"/>
-      <c r="G905" s="8"/>
-    </row>
-    <row r="906">
-      <c r="B906" s="16"/>
-      <c r="C906" s="8"/>
-      <c r="D906" s="11"/>
-      <c r="E906" s="8"/>
-      <c r="F906" s="8"/>
-      <c r="G906" s="8"/>
-    </row>
-    <row r="907">
-      <c r="B907" s="16"/>
-      <c r="C907" s="8"/>
-      <c r="D907" s="11"/>
-      <c r="E907" s="8"/>
-      <c r="F907" s="8"/>
-      <c r="G907" s="8"/>
-    </row>
-    <row r="908">
-      <c r="B908" s="16"/>
-      <c r="C908" s="8"/>
-      <c r="D908" s="11"/>
-      <c r="E908" s="8"/>
-      <c r="F908" s="8"/>
-      <c r="G908" s="8"/>
-    </row>
-    <row r="909">
-      <c r="B909" s="16"/>
-      <c r="C909" s="8"/>
-      <c r="D909" s="11"/>
-      <c r="E909" s="8"/>
-      <c r="F909" s="8"/>
-      <c r="G909" s="8"/>
-    </row>
-    <row r="910">
-      <c r="B910" s="16"/>
-      <c r="C910" s="8"/>
-      <c r="D910" s="11"/>
-      <c r="E910" s="8"/>
-      <c r="F910" s="8"/>
-      <c r="G910" s="8"/>
-    </row>
-    <row r="911">
-      <c r="B911" s="16"/>
-      <c r="C911" s="8"/>
-      <c r="D911" s="11"/>
-      <c r="E911" s="8"/>
-      <c r="F911" s="8"/>
-      <c r="G911" s="8"/>
-    </row>
-    <row r="912">
-      <c r="B912" s="16"/>
-      <c r="C912" s="8"/>
-      <c r="D912" s="11"/>
-      <c r="E912" s="8"/>
-      <c r="F912" s="8"/>
-      <c r="G912" s="8"/>
-    </row>
-    <row r="913">
-      <c r="B913" s="16"/>
-      <c r="C913" s="8"/>
-      <c r="D913" s="11"/>
-      <c r="E913" s="8"/>
-      <c r="F913" s="8"/>
-      <c r="G913" s="8"/>
-    </row>
-    <row r="914">
-      <c r="B914" s="16"/>
-      <c r="C914" s="8"/>
-      <c r="D914" s="11"/>
-      <c r="E914" s="8"/>
-      <c r="F914" s="8"/>
-      <c r="G914" s="8"/>
-    </row>
-    <row r="915">
-      <c r="B915" s="16"/>
-      <c r="C915" s="8"/>
-      <c r="D915" s="11"/>
-      <c r="E915" s="8"/>
-      <c r="F915" s="8"/>
-      <c r="G915" s="8"/>
-    </row>
-    <row r="916">
-      <c r="B916" s="16"/>
-      <c r="C916" s="8"/>
-      <c r="D916" s="11"/>
-      <c r="E916" s="8"/>
-      <c r="F916" s="8"/>
-      <c r="G916" s="8"/>
-    </row>
-    <row r="917">
-      <c r="B917" s="16"/>
-      <c r="C917" s="8"/>
-      <c r="D917" s="11"/>
-      <c r="E917" s="8"/>
-      <c r="F917" s="8"/>
-      <c r="G917" s="8"/>
-    </row>
-    <row r="918">
-      <c r="B918" s="16"/>
-      <c r="C918" s="8"/>
-      <c r="D918" s="11"/>
-      <c r="E918" s="8"/>
-      <c r="F918" s="8"/>
-      <c r="G918" s="8"/>
-    </row>
-    <row r="919">
-      <c r="B919" s="16"/>
-      <c r="C919" s="8"/>
-      <c r="D919" s="11"/>
-      <c r="E919" s="8"/>
-      <c r="F919" s="8"/>
-      <c r="G919" s="8"/>
-    </row>
-    <row r="920">
-      <c r="B920" s="16"/>
-      <c r="C920" s="8"/>
-      <c r="D920" s="11"/>
-      <c r="E920" s="8"/>
-      <c r="F920" s="8"/>
-      <c r="G920" s="8"/>
-    </row>
-    <row r="921">
-      <c r="B921" s="16"/>
-      <c r="C921" s="8"/>
-      <c r="D921" s="11"/>
-      <c r="E921" s="8"/>
-      <c r="F921" s="8"/>
-      <c r="G921" s="8"/>
-    </row>
-    <row r="922">
-      <c r="B922" s="16"/>
-      <c r="C922" s="8"/>
-      <c r="D922" s="11"/>
-      <c r="E922" s="8"/>
-      <c r="F922" s="8"/>
-      <c r="G922" s="8"/>
-    </row>
-    <row r="923">
-      <c r="B923" s="16"/>
-      <c r="C923" s="8"/>
-      <c r="D923" s="11"/>
-      <c r="E923" s="8"/>
-      <c r="F923" s="8"/>
-      <c r="G923" s="8"/>
-    </row>
-    <row r="924">
-      <c r="B924" s="16"/>
-      <c r="C924" s="8"/>
-      <c r="D924" s="11"/>
-      <c r="E924" s="8"/>
-      <c r="F924" s="8"/>
-      <c r="G924" s="8"/>
-    </row>
-    <row r="925">
-      <c r="B925" s="16"/>
-      <c r="C925" s="8"/>
-      <c r="D925" s="11"/>
-      <c r="E925" s="8"/>
-      <c r="F925" s="8"/>
-      <c r="G925" s="8"/>
-    </row>
-    <row r="926">
-      <c r="B926" s="16"/>
-      <c r="C926" s="8"/>
-      <c r="D926" s="11"/>
-      <c r="E926" s="8"/>
-      <c r="F926" s="8"/>
-      <c r="G926" s="8"/>
-    </row>
-    <row r="927">
-      <c r="B927" s="16"/>
-      <c r="C927" s="8"/>
-      <c r="D927" s="11"/>
-      <c r="E927" s="8"/>
-      <c r="F927" s="8"/>
-      <c r="G927" s="8"/>
-    </row>
-    <row r="928">
-      <c r="B928" s="16"/>
-      <c r="C928" s="8"/>
-      <c r="D928" s="11"/>
-      <c r="E928" s="8"/>
-      <c r="F928" s="8"/>
-      <c r="G928" s="8"/>
-    </row>
-    <row r="929">
-      <c r="B929" s="16"/>
-      <c r="C929" s="8"/>
-      <c r="D929" s="11"/>
-      <c r="E929" s="8"/>
-      <c r="F929" s="8"/>
-      <c r="G929" s="8"/>
-    </row>
-    <row r="930">
-      <c r="B930" s="16"/>
-      <c r="C930" s="8"/>
-      <c r="D930" s="11"/>
-      <c r="E930" s="8"/>
-      <c r="F930" s="8"/>
-      <c r="G930" s="8"/>
-    </row>
-    <row r="931">
-      <c r="B931" s="16"/>
-      <c r="C931" s="8"/>
-      <c r="D931" s="11"/>
-      <c r="E931" s="8"/>
-      <c r="F931" s="8"/>
-      <c r="G931" s="8"/>
-    </row>
-    <row r="932">
-      <c r="B932" s="16"/>
-      <c r="C932" s="8"/>
-      <c r="D932" s="11"/>
-      <c r="E932" s="8"/>
-      <c r="F932" s="8"/>
-      <c r="G932" s="8"/>
-    </row>
-    <row r="933">
-      <c r="B933" s="16"/>
-      <c r="C933" s="8"/>
-      <c r="D933" s="11"/>
-      <c r="E933" s="8"/>
-      <c r="F933" s="8"/>
-      <c r="G933" s="8"/>
-    </row>
-    <row r="934">
-      <c r="B934" s="16"/>
-      <c r="C934" s="8"/>
-      <c r="D934" s="11"/>
-      <c r="E934" s="8"/>
-      <c r="F934" s="8"/>
-      <c r="G934" s="8"/>
-    </row>
-    <row r="935">
-      <c r="B935" s="16"/>
-      <c r="C935" s="8"/>
-      <c r="D935" s="11"/>
-      <c r="E935" s="8"/>
-      <c r="F935" s="8"/>
-      <c r="G935" s="8"/>
-    </row>
-    <row r="936">
-      <c r="B936" s="16"/>
-      <c r="C936" s="8"/>
-      <c r="D936" s="11"/>
-      <c r="E936" s="8"/>
-      <c r="F936" s="8"/>
-      <c r="G936" s="8"/>
-    </row>
-    <row r="937">
-      <c r="B937" s="16"/>
-      <c r="C937" s="8"/>
-      <c r="D937" s="11"/>
-      <c r="E937" s="8"/>
-      <c r="F937" s="8"/>
-      <c r="G937" s="8"/>
-    </row>
-    <row r="938">
-      <c r="B938" s="16"/>
-      <c r="C938" s="8"/>
-      <c r="D938" s="11"/>
-      <c r="E938" s="8"/>
-      <c r="F938" s="8"/>
-      <c r="G938" s="8"/>
-    </row>
-    <row r="939">
-      <c r="B939" s="16"/>
-      <c r="C939" s="8"/>
-      <c r="D939" s="11"/>
-      <c r="E939" s="8"/>
-      <c r="F939" s="8"/>
-      <c r="G939" s="8"/>
-    </row>
-    <row r="940">
-      <c r="B940" s="16"/>
-      <c r="C940" s="8"/>
-      <c r="D940" s="11"/>
-      <c r="E940" s="8"/>
-      <c r="F940" s="8"/>
-      <c r="G940" s="8"/>
-    </row>
-    <row r="941">
-      <c r="B941" s="16"/>
-      <c r="C941" s="8"/>
-      <c r="D941" s="11"/>
-      <c r="E941" s="8"/>
-      <c r="F941" s="8"/>
-      <c r="G941" s="8"/>
-    </row>
-    <row r="942">
-      <c r="B942" s="16"/>
-      <c r="C942" s="8"/>
-      <c r="D942" s="11"/>
-      <c r="E942" s="8"/>
-      <c r="F942" s="8"/>
-      <c r="G942" s="8"/>
-    </row>
-    <row r="943">
-      <c r="B943" s="16"/>
-      <c r="C943" s="8"/>
-      <c r="D943" s="11"/>
-      <c r="E943" s="8"/>
-      <c r="F943" s="8"/>
-      <c r="G943" s="8"/>
-    </row>
-    <row r="944">
-      <c r="B944" s="16"/>
-      <c r="C944" s="8"/>
-      <c r="D944" s="11"/>
-      <c r="E944" s="8"/>
-      <c r="F944" s="8"/>
-      <c r="G944" s="8"/>
-    </row>
-    <row r="945">
-      <c r="B945" s="16"/>
-      <c r="C945" s="8"/>
-      <c r="D945" s="11"/>
-      <c r="E945" s="8"/>
-      <c r="F945" s="8"/>
-      <c r="G945" s="8"/>
-    </row>
-    <row r="946">
-      <c r="B946" s="16"/>
-      <c r="C946" s="8"/>
-      <c r="D946" s="11"/>
-      <c r="E946" s="8"/>
-      <c r="F946" s="8"/>
-      <c r="G946" s="8"/>
-    </row>
-    <row r="947">
-      <c r="B947" s="16"/>
-      <c r="C947" s="8"/>
-      <c r="D947" s="11"/>
-      <c r="E947" s="8"/>
-      <c r="F947" s="8"/>
-      <c r="G947" s="8"/>
-    </row>
-    <row r="948">
-      <c r="B948" s="16"/>
-      <c r="C948" s="8"/>
-      <c r="D948" s="11"/>
-      <c r="E948" s="8"/>
-      <c r="F948" s="8"/>
-      <c r="G948" s="8"/>
-    </row>
-    <row r="949">
-      <c r="B949" s="16"/>
-      <c r="C949" s="8"/>
-      <c r="D949" s="11"/>
-      <c r="E949" s="8"/>
-      <c r="F949" s="8"/>
-      <c r="G949" s="8"/>
-    </row>
-    <row r="950">
-      <c r="B950" s="16"/>
-      <c r="C950" s="8"/>
-      <c r="D950" s="11"/>
-      <c r="E950" s="8"/>
-      <c r="F950" s="8"/>
-      <c r="G950" s="8"/>
-    </row>
-    <row r="951">
-      <c r="B951" s="16"/>
-      <c r="C951" s="8"/>
-      <c r="D951" s="11"/>
-      <c r="E951" s="8"/>
-      <c r="F951" s="8"/>
-      <c r="G951" s="8"/>
-    </row>
-    <row r="952">
-      <c r="B952" s="16"/>
-      <c r="C952" s="8"/>
-      <c r="D952" s="11"/>
-      <c r="E952" s="8"/>
-      <c r="F952" s="8"/>
-      <c r="G952" s="8"/>
-    </row>
-    <row r="953">
-      <c r="B953" s="16"/>
-      <c r="C953" s="8"/>
-      <c r="D953" s="11"/>
-      <c r="E953" s="8"/>
-      <c r="F953" s="8"/>
-      <c r="G953" s="8"/>
-    </row>
-    <row r="954">
-      <c r="B954" s="16"/>
-      <c r="C954" s="8"/>
-      <c r="D954" s="11"/>
-      <c r="E954" s="8"/>
-      <c r="F954" s="8"/>
-      <c r="G954" s="8"/>
-    </row>
-    <row r="955">
-      <c r="B955" s="16"/>
-      <c r="C955" s="8"/>
-      <c r="D955" s="11"/>
-      <c r="E955" s="8"/>
-      <c r="F955" s="8"/>
-      <c r="G955" s="8"/>
-    </row>
-    <row r="956">
-      <c r="B956" s="16"/>
-      <c r="C956" s="8"/>
-      <c r="D956" s="11"/>
-      <c r="E956" s="8"/>
-      <c r="F956" s="8"/>
-      <c r="G956" s="8"/>
-    </row>
-    <row r="957">
-      <c r="B957" s="16"/>
-      <c r="C957" s="8"/>
-      <c r="D957" s="11"/>
-      <c r="E957" s="8"/>
-      <c r="F957" s="8"/>
-      <c r="G957" s="8"/>
-    </row>
-    <row r="958">
-      <c r="B958" s="16"/>
-      <c r="C958" s="8"/>
-      <c r="D958" s="11"/>
-      <c r="E958" s="8"/>
-      <c r="F958" s="8"/>
-      <c r="G958" s="8"/>
-    </row>
-    <row r="959">
-      <c r="B959" s="16"/>
-      <c r="C959" s="8"/>
-      <c r="D959" s="11"/>
-      <c r="E959" s="8"/>
-      <c r="F959" s="8"/>
-      <c r="G959" s="8"/>
-    </row>
-    <row r="960">
-      <c r="B960" s="16"/>
-      <c r="C960" s="8"/>
-      <c r="D960" s="11"/>
-      <c r="E960" s="8"/>
-      <c r="F960" s="8"/>
-      <c r="G960" s="8"/>
-    </row>
-    <row r="961">
-      <c r="B961" s="16"/>
-      <c r="C961" s="8"/>
-      <c r="D961" s="11"/>
-      <c r="E961" s="8"/>
-      <c r="F961" s="8"/>
-      <c r="G961" s="8"/>
-    </row>
-    <row r="962">
-      <c r="B962" s="16"/>
-      <c r="C962" s="8"/>
-      <c r="D962" s="11"/>
-      <c r="E962" s="8"/>
-      <c r="F962" s="8"/>
-      <c r="G962" s="8"/>
-    </row>
-    <row r="963">
-      <c r="B963" s="16"/>
-      <c r="C963" s="8"/>
-      <c r="D963" s="11"/>
-      <c r="E963" s="8"/>
-      <c r="F963" s="8"/>
-      <c r="G963" s="8"/>
-    </row>
-    <row r="964">
-      <c r="B964" s="16"/>
-      <c r="C964" s="8"/>
-      <c r="D964" s="11"/>
-      <c r="E964" s="8"/>
-      <c r="F964" s="8"/>
-      <c r="G964" s="8"/>
-    </row>
-    <row r="965">
-      <c r="B965" s="16"/>
-      <c r="C965" s="8"/>
-      <c r="D965" s="11"/>
-      <c r="E965" s="8"/>
-      <c r="F965" s="8"/>
-      <c r="G965" s="8"/>
-    </row>
-    <row r="966">
-      <c r="B966" s="16"/>
-      <c r="C966" s="8"/>
-      <c r="D966" s="11"/>
-      <c r="E966" s="8"/>
-      <c r="F966" s="8"/>
-      <c r="G966" s="8"/>
-    </row>
-    <row r="967">
-      <c r="B967" s="16"/>
-      <c r="C967" s="8"/>
-      <c r="D967" s="11"/>
-      <c r="E967" s="8"/>
-      <c r="F967" s="8"/>
-      <c r="G967" s="8"/>
-    </row>
-    <row r="968">
-      <c r="B968" s="16"/>
-      <c r="C968" s="8"/>
-      <c r="D968" s="11"/>
-      <c r="E968" s="8"/>
-      <c r="F968" s="8"/>
-      <c r="G968" s="8"/>
-    </row>
-    <row r="969">
-      <c r="B969" s="16"/>
-      <c r="C969" s="8"/>
-      <c r="D969" s="11"/>
-      <c r="E969" s="8"/>
-      <c r="F969" s="8"/>
-      <c r="G969" s="8"/>
-    </row>
-    <row r="970">
-      <c r="B970" s="16"/>
-      <c r="C970" s="8"/>
-      <c r="D970" s="11"/>
-      <c r="E970" s="8"/>
-      <c r="F970" s="8"/>
-      <c r="G970" s="8"/>
-    </row>
-    <row r="971">
-      <c r="B971" s="16"/>
-      <c r="C971" s="8"/>
-      <c r="D971" s="11"/>
-      <c r="E971" s="8"/>
-      <c r="F971" s="8"/>
-      <c r="G971" s="8"/>
-    </row>
-    <row r="972">
-      <c r="B972" s="16"/>
-      <c r="C972" s="8"/>
-      <c r="D972" s="11"/>
-      <c r="E972" s="8"/>
-      <c r="F972" s="8"/>
-      <c r="G972" s="8"/>
-    </row>
-    <row r="973">
-      <c r="B973" s="16"/>
-      <c r="C973" s="8"/>
-      <c r="D973" s="11"/>
-      <c r="E973" s="8"/>
-      <c r="F973" s="8"/>
-      <c r="G973" s="8"/>
-    </row>
-    <row r="974">
-      <c r="B974" s="16"/>
-      <c r="C974" s="8"/>
-      <c r="D974" s="11"/>
-      <c r="E974" s="8"/>
-      <c r="F974" s="8"/>
-      <c r="G974" s="8"/>
-    </row>
-    <row r="975">
-      <c r="B975" s="16"/>
-      <c r="C975" s="8"/>
-      <c r="D975" s="11"/>
-      <c r="E975" s="8"/>
-      <c r="F975" s="8"/>
-      <c r="G975" s="8"/>
-    </row>
-    <row r="976">
-      <c r="B976" s="16"/>
-      <c r="C976" s="8"/>
-      <c r="D976" s="11"/>
-      <c r="E976" s="8"/>
-      <c r="F976" s="8"/>
-      <c r="G976" s="8"/>
-    </row>
-    <row r="977">
-      <c r="B977" s="16"/>
-      <c r="C977" s="8"/>
-      <c r="D977" s="11"/>
-      <c r="E977" s="8"/>
-      <c r="F977" s="8"/>
-      <c r="G977" s="8"/>
-    </row>
-    <row r="978">
-      <c r="B978" s="16"/>
-      <c r="C978" s="8"/>
-      <c r="D978" s="11"/>
-      <c r="E978" s="8"/>
-      <c r="F978" s="8"/>
-      <c r="G978" s="8"/>
-    </row>
-    <row r="979">
-      <c r="B979" s="16"/>
-      <c r="C979" s="8"/>
-      <c r="D979" s="11"/>
-      <c r="E979" s="8"/>
-      <c r="F979" s="8"/>
-      <c r="G979" s="8"/>
-    </row>
-    <row r="980">
-      <c r="B980" s="16"/>
-      <c r="C980" s="8"/>
-      <c r="D980" s="11"/>
-      <c r="E980" s="8"/>
-      <c r="F980" s="8"/>
-      <c r="G980" s="8"/>
-    </row>
-    <row r="981">
-      <c r="B981" s="16"/>
-      <c r="C981" s="8"/>
-      <c r="D981" s="11"/>
-      <c r="E981" s="8"/>
-      <c r="F981" s="8"/>
-      <c r="G981" s="8"/>
-    </row>
-    <row r="982">
-      <c r="B982" s="16"/>
-      <c r="C982" s="8"/>
-      <c r="D982" s="11"/>
-      <c r="E982" s="8"/>
-      <c r="F982" s="8"/>
-      <c r="G982" s="8"/>
-    </row>
-    <row r="983">
-      <c r="B983" s="16"/>
-      <c r="C983" s="8"/>
-      <c r="D983" s="11"/>
-      <c r="E983" s="8"/>
-      <c r="F983" s="8"/>
-      <c r="G983" s="8"/>
-    </row>
-    <row r="984">
-      <c r="B984" s="16"/>
-      <c r="C984" s="8"/>
-      <c r="D984" s="11"/>
-      <c r="E984" s="8"/>
-      <c r="F984" s="8"/>
-      <c r="G984" s="8"/>
-    </row>
-    <row r="985">
-      <c r="B985" s="16"/>
-      <c r="C985" s="8"/>
-      <c r="D985" s="11"/>
-      <c r="E985" s="8"/>
-      <c r="F985" s="8"/>
-      <c r="G985" s="8"/>
-    </row>
-    <row r="986">
-      <c r="B986" s="16"/>
-      <c r="C986" s="8"/>
-      <c r="D986" s="11"/>
-      <c r="E986" s="8"/>
-      <c r="F986" s="8"/>
-      <c r="G986" s="8"/>
-    </row>
-    <row r="987">
-      <c r="B987" s="16"/>
-      <c r="C987" s="8"/>
-      <c r="D987" s="11"/>
-      <c r="E987" s="8"/>
-      <c r="F987" s="8"/>
-      <c r="G987" s="8"/>
-    </row>
-    <row r="988">
-      <c r="B988" s="16"/>
-      <c r="C988" s="8"/>
-      <c r="D988" s="11"/>
-      <c r="E988" s="8"/>
-      <c r="F988" s="8"/>
-      <c r="G988" s="8"/>
-    </row>
-    <row r="989">
-      <c r="B989" s="16"/>
-      <c r="C989" s="8"/>
-      <c r="D989" s="11"/>
-      <c r="E989" s="8"/>
-      <c r="F989" s="8"/>
-      <c r="G989" s="8"/>
-    </row>
-    <row r="990">
-      <c r="B990" s="16"/>
-      <c r="C990" s="8"/>
-      <c r="D990" s="11"/>
-      <c r="E990" s="8"/>
-      <c r="F990" s="8"/>
-      <c r="G990" s="8"/>
-    </row>
-    <row r="991">
-      <c r="B991" s="16"/>
-      <c r="C991" s="8"/>
-      <c r="D991" s="11"/>
-      <c r="E991" s="8"/>
-      <c r="F991" s="8"/>
-      <c r="G991" s="8"/>
-    </row>
-    <row r="992">
-      <c r="B992" s="16"/>
-      <c r="C992" s="8"/>
-      <c r="D992" s="11"/>
-      <c r="E992" s="8"/>
-      <c r="F992" s="8"/>
-      <c r="G992" s="8"/>
-    </row>
-    <row r="993">
-      <c r="B993" s="16"/>
-      <c r="C993" s="8"/>
-      <c r="D993" s="11"/>
-      <c r="E993" s="8"/>
-      <c r="F993" s="8"/>
-      <c r="G993" s="8"/>
-    </row>
-    <row r="994">
-      <c r="B994" s="16"/>
-      <c r="C994" s="8"/>
-      <c r="D994" s="11"/>
-      <c r="E994" s="8"/>
-      <c r="F994" s="8"/>
-      <c r="G994" s="8"/>
-    </row>
-    <row r="995">
-      <c r="B995" s="16"/>
-      <c r="C995" s="8"/>
-      <c r="D995" s="11"/>
-      <c r="E995" s="8"/>
-      <c r="F995" s="8"/>
-      <c r="G995" s="8"/>
-    </row>
-    <row r="996">
-      <c r="B996" s="16"/>
-      <c r="C996" s="8"/>
-      <c r="D996" s="11"/>
-      <c r="E996" s="8"/>
-      <c r="F996" s="8"/>
-      <c r="G996" s="8"/>
-    </row>
-    <row r="997">
-      <c r="B997" s="16"/>
-      <c r="C997" s="8"/>
-      <c r="D997" s="11"/>
-      <c r="E997" s="8"/>
-      <c r="F997" s="8"/>
-      <c r="G997" s="8"/>
-    </row>
-    <row r="998">
-      <c r="B998" s="16"/>
-      <c r="C998" s="8"/>
-      <c r="D998" s="11"/>
-      <c r="E998" s="8"/>
-      <c r="F998" s="8"/>
-      <c r="G998" s="8"/>
-    </row>
-    <row r="999">
-      <c r="B999" s="16"/>
-      <c r="C999" s="8"/>
-      <c r="D999" s="11"/>
-      <c r="E999" s="8"/>
-      <c r="F999" s="8"/>
-      <c r="G999" s="8"/>
-    </row>
-    <row r="1000">
-      <c r="B1000" s="16"/>
-      <c r="C1000" s="8"/>
-      <c r="D1000" s="11"/>
-      <c r="E1000" s="8"/>
-      <c r="F1000" s="8"/>
-      <c r="G1000" s="8"/>
-    </row>
-    <row r="1001">
-      <c r="B1001" s="16"/>
-      <c r="C1001" s="8"/>
-      <c r="D1001" s="11"/>
-      <c r="E1001" s="8"/>
-      <c r="F1001" s="8"/>
-      <c r="G1001" s="8"/>
-    </row>
-    <row r="1002">
-      <c r="B1002" s="16"/>
-      <c r="C1002" s="8"/>
-      <c r="D1002" s="11"/>
-      <c r="E1002" s="8"/>
-      <c r="F1002" s="8"/>
-      <c r="G1002" s="8"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" location="90591a250/=xst4ec" ref="C5"/>
-    <hyperlink r:id="rId2" location="90576a102/=xsshuh" ref="C6"/>
-    <hyperlink r:id="rId3" location="91166a210/=xsshhz" ref="C7"/>
-    <hyperlink r:id="rId4" ref="C9"/>
-    <hyperlink r:id="rId5" ref="C12"/>
-    <hyperlink r:id="rId6" ref="C19"/>
-    <hyperlink r:id="rId7" location="product-description-iframe" ref="C20"/>
-    <hyperlink r:id="rId8" ref="C21"/>
-    <hyperlink r:id="rId9" ref="C22"/>
-    <hyperlink r:id="rId10" ref="C23"/>
-    <hyperlink r:id="rId11" ref="C24"/>
-    <hyperlink r:id="rId12" ref="C25"/>
+    <hyperlink r:id="rId1" location="90591a250/=xst4ec" ref="C7"/>
+    <hyperlink r:id="rId2" location="90576a102/=xsshuh" ref="C8"/>
+    <hyperlink r:id="rId3" location="91166a210/=xsshhz" ref="C9"/>
+    <hyperlink r:id="rId4" ref="C11"/>
+    <hyperlink r:id="rId5" ref="C14"/>
+    <hyperlink r:id="rId6" ref="C16"/>
+    <hyperlink r:id="rId7" ref="C21"/>
+    <hyperlink r:id="rId8" location="product-description-iframe" ref="C22"/>
+    <hyperlink r:id="rId9" ref="C23"/>
+    <hyperlink r:id="rId10" ref="C24"/>
+    <hyperlink r:id="rId11" ref="C25"/>
+    <hyperlink r:id="rId12" ref="C26"/>
+    <hyperlink r:id="rId13" ref="C27"/>
+    <hyperlink r:id="rId14" ref="C28"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>